<commit_message>
Build Excel template from script
</commit_message>
<xml_diff>
--- a/contribute/template.xlsx
+++ b/contribute/template.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="borehole" sheetId="1" r:id="rId1"/>
     <sheet name="measurement" sheetId="2" r:id="rId2"/>
-    <sheet name="enum.drill_method" sheetId="3" state="hidden" r:id="rId3"/>
+    <sheet name="lists" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -30,13 +30,12 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">[integer] 
+          <t>[integer] id
 Unique identifier.
 constraints:
-- required: True
-- unique: True
-- minimum: 1
-</t>
+  - required: True
+  - unique: True
+  - minimum: 1</t>
         </r>
       </text>
     </comment>
@@ -49,12 +48,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">[string] 
+          <t>[string] glacier_name
 Glacier or ice cap name (as reported).
 constraints:
-- required: True
-- pattern: [^\s]+( [^\s]+)*
-</t>
+  - required: True
+  - pattern: [^\s]+( [^\s]+)*</t>
         </r>
       </text>
     </comment>
@@ -67,11 +65,10 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">[string] 
+          <t>[string] glims_id
 Global Land Ice Measurements from Space (GLIMS) glacier identifier.
 constraints:
-- pattern: G[0-9]{6}E[0-9]{5}[NS]
-</t>
+  - pattern: G[0-9]{6}E[0-9]{5}[NS]</t>
         </r>
       </text>
     </comment>
@@ -84,13 +81,12 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">[number] 
+          <t>[number: degree] latitude
 Latitude (EPSG 4326).
 constraints:
-- required: True
-- minimum: -90
-- maximum: 90
-</t>
+  - required: True
+  - minimum: -90
+  - maximum: 90</t>
         </r>
       </text>
     </comment>
@@ -103,13 +99,12 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">[number] 
+          <t>[number: degree] longitude
 Longitude (EPSG 4326).
 constraints:
-- required: True
-- minimum: -180
-- maximum: 180
-</t>
+  - required: True
+  - minimum: -180
+  - maximum: 180</t>
         </r>
       </text>
     </comment>
@@ -122,12 +117,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">[number] 
+          <t>[number: m] elevation
 Elevation above sea level.
 constraints:
-- required: True
-- maximum: 9999.0
-</t>
+  - required: True
+  - maximum: 9999.0</t>
         </r>
       </text>
     </comment>
@@ -140,9 +134,8 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">[string] 
-Borehole name (e.g. as labeled on a plot).
-</t>
+          <t>[string] label
+Borehole name (e.g. as labeled on a plot).</t>
         </r>
       </text>
     </comment>
@@ -155,9 +148,9 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">[date] 
-Drilling date, or if not known precisely, the first possible date (e.g. 2019 → 2019-01-01).
-</t>
+          <t>[date] date_min
+Begin date of drilling, or if not known precisely, the first possible date (e.g. 2019 → 2019-01-01).
+format: %Y-%m-%d</t>
         </r>
       </text>
     </comment>
@@ -170,9 +163,9 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">[date] 
-Drilling date, or if not known precisely, the last possible date (e.g. 2019 → 2019-12-31).
-</t>
+          <t>[date] date_max
+End date of drilling, or if not known precisely, the last possible date (e.g. 2019 → 2019-12-31).
+format: %Y-%m-%d</t>
         </r>
       </text>
     </comment>
@@ -185,14 +178,13 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">[string] 
+          <t>[string] drill_method
 Drilling method:
-- mechanical
-- thermal: Hot water or steam
+- mechanical: Push, percussion, rotary, ...
+- thermal: Hot point, electrothermal, steam, ...
 - combined: Mechanical and thermal
 constraints:
-- enum: ['mechanical', 'thermal', 'combined']
-</t>
+  - enum: ['mechanical', 'thermal', 'combined']</t>
         </r>
       </text>
     </comment>
@@ -205,9 +197,8 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">[number] 
-Starting depth of ice. Infinity (INF) indicates that ice was not reached.
-</t>
+          <t>[number: m] ice_depth
+Starting depth of ice. Infinity (INF) indicates that ice was not reached.</t>
         </r>
       </text>
     </comment>
@@ -220,9 +211,8 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">[number] 
-Total borehole depth (not including drilling in the underlying bed).
-</t>
+          <t>[number: m] depth
+Total borehole depth (not including drilling in the underlying bed).</t>
         </r>
       </text>
     </comment>
@@ -235,9 +225,8 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">[boolean] 
-Whether the borehole reached the glacier bed.
-</t>
+          <t>[boolean] to_bed
+Whether the borehole reached the glacier bed.</t>
         </r>
       </text>
     </comment>
@@ -250,9 +239,8 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">[number] 
-Thermistor accuracy or precision (as reported). Typically understood to represent one standard deviation.
-</t>
+          <t>[number: °C] temperature_accuracy
+Thermistor accuracy or precision (as reported). Typically understood to represent one standard deviation.</t>
         </r>
       </text>
     </comment>
@@ -265,11 +253,10 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">[string] 
+          <t>[string] notes
 Additional remarks about the study site, the borehole, or the measurements therein. Literature references should be formatted as `{url}` or `{author} {year} ({url})`.
 constraints:
-- pattern: [^\s]+( [^\s]+)*
-</t>
+  - pattern: [^\s]+( [^\s]+)*</t>
         </r>
       </text>
     </comment>
@@ -292,11 +279,10 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">[integer] 
+          <t>[integer] borehole_id
 Borehole identifier.
 constraints:
-- required: True
-</t>
+  - required: True</t>
         </r>
       </text>
     </comment>
@@ -309,11 +295,10 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">[number] 
+          <t>[number: m] depth
 Depth below the glacier surface.
 constraints:
-- required: True
-</t>
+  - required: True</t>
         </r>
       </text>
     </comment>
@@ -326,11 +311,10 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">[number] 
+          <t>[number: °C] temperature
 Temperature.
 constraints:
-- required: True
-</t>
+  - required: True</t>
         </r>
       </text>
     </comment>
@@ -343,9 +327,9 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">[date] 
+          <t>[date] date_min
 Measurement date, or if not known precisely, the first possible date (e.g. 2019 → 2019-01-01).
-</t>
+format: %Y-%m-%d</t>
         </r>
       </text>
     </comment>
@@ -358,11 +342,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">[date] 
+          <t>[date] date_max
 Measurement date, or if not known precisely, the last possible date (e.g. 2019 → 2019-12-31).
-constraints:
-- required: True
-</t>
+format: %Y-%m-%d
+constraints:
+  - required: True</t>
         </r>
       </text>
     </comment>
@@ -375,9 +359,9 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">[time] 
+          <t>[time] time
 Measurement time.
-</t>
+format: %H:%M:%S</t>
         </r>
       </text>
     </comment>
@@ -390,9 +374,8 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">[boolean] 
-Whether `time` is in Coordinated Universal Time (True) or in another (but unknown) timezone (False).
-</t>
+          <t>[number: h] utc_offset
+Time offset relative to Coordinated Universal Time (UTC).</t>
         </r>
       </text>
     </comment>
@@ -405,9 +388,8 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">[boolean] 
-Whether the profile is in thermal equilibrium following drilling.
-</t>
+          <t>[boolean] equilibrated
+Whether temperatures have equilibrated following drilling.</t>
         </r>
       </text>
     </comment>
@@ -472,7 +454,7 @@
     <t>time</t>
   </si>
   <si>
-    <t>utc</t>
+    <t>utc_offset</t>
   </si>
   <si>
     <t>equilibrated</t>
@@ -864,7 +846,6 @@
     <col min="12" max="13" width="10.7109375" customWidth="1"/>
     <col min="14" max="14" width="24.7109375" customWidth="1"/>
     <col min="15" max="15" width="10.7109375" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -917,59 +898,59 @@
   </sheetData>
   <conditionalFormatting sqref="A2:A1048576">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>OR(AND(ISBLANK(A2),COUNTBLANK($A2:$O2)&lt;&gt;15),IF(ISBLANK(A2),FALSE,OR(IF(ISNUMBER(A2),INT(A2)&lt;&gt;A2,TRUE),COUNTIF(A$2:A$1048576,A2)&gt;=2,A2&lt;1)))</formula>
+      <formula>OR(AND(ISBLANK(A2), COUNTBLANK($A2:$O2) &lt;&gt; 15), IF(ISBLANK(A2), FALSE, OR(IF(ISNUMBER(A2), INT(A2) &lt;&gt; A2, TRUE), COUNTIF(A$2:A$1048576, A2) &gt;= 2, A2 &lt; 1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B1048576">
     <cfRule type="expression" dxfId="0" priority="2">
-      <formula>AND(ISBLANK(B2),COUNTBLANK($A2:$O2)&lt;&gt;15)</formula>
+      <formula>AND(ISBLANK(B2), COUNTBLANK($A2:$O2) &lt;&gt; 15)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D1048576">
     <cfRule type="expression" dxfId="0" priority="3">
-      <formula>OR(AND(ISBLANK(D2),COUNTBLANK($A2:$O2)&lt;&gt;15),IF(ISBLANK(D2),FALSE,OR(NOT(ISNUMBER(D2)),D2&lt;-90,D2&gt;90)))</formula>
+      <formula>OR(AND(ISBLANK(D2), COUNTBLANK($A2:$O2) &lt;&gt; 15), IF(ISBLANK(D2), FALSE, OR(NOT(ISNUMBER(D2)), D2 &lt; -90, D2 &gt; 90)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E1048576">
     <cfRule type="expression" dxfId="0" priority="4">
-      <formula>OR(AND(ISBLANK(E2),COUNTBLANK($A2:$O2)&lt;&gt;15),IF(ISBLANK(E2),FALSE,OR(NOT(ISNUMBER(E2)),E2&lt;-180,E2&gt;180)))</formula>
+      <formula>OR(AND(ISBLANK(E2), COUNTBLANK($A2:$O2) &lt;&gt; 15), IF(ISBLANK(E2), FALSE, OR(NOT(ISNUMBER(E2)), E2 &lt; -180, E2 &gt; 180)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F1048576">
     <cfRule type="expression" dxfId="0" priority="5">
-      <formula>OR(AND(ISBLANK(F2),COUNTBLANK($A2:$O2)&lt;&gt;15),IF(ISBLANK(F2),FALSE,OR(NOT(ISNUMBER(F2)),F2&gt;9999.0)))</formula>
+      <formula>OR(AND(ISBLANK(F2), COUNTBLANK($A2:$O2) &lt;&gt; 15), IF(ISBLANK(F2), FALSE, OR(NOT(ISNUMBER(F2)), F2 &gt; 9999.0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J1048576">
     <cfRule type="expression" dxfId="0" priority="6">
-      <formula>IF(ISBLANK(J2),FALSE,ISNA(MATCH(J2,'enum.drill_method'!$A$1:$A$3,0)))</formula>
+      <formula>IF(ISBLANK(J2), FALSE, ISNA(MATCH(J2, 'lists'!$A$1:$A$3, 0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K1048576">
     <cfRule type="expression" dxfId="0" priority="7">
-      <formula>IF(ISBLANK(K2),FALSE,NOT(ISNUMBER(K2)))</formula>
+      <formula>IF(ISBLANK(K2), FALSE, NOT(ISNUMBER(K2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L1048576">
     <cfRule type="expression" dxfId="0" priority="8">
-      <formula>IF(ISBLANK(L2),FALSE,NOT(ISNUMBER(L2)))</formula>
+      <formula>IF(ISBLANK(L2), FALSE, NOT(ISNUMBER(L2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M1048576">
     <cfRule type="expression" dxfId="0" priority="9">
-      <formula>IF(ISBLANK(M2),FALSE,AND(M2&lt;&gt;TRUE,M2&lt;&gt;FALSE))</formula>
+      <formula>IF(ISBLANK(M2), FALSE, AND(M2 &lt;&gt; TRUE, M2 &lt;&gt; FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N1048576">
     <cfRule type="expression" dxfId="0" priority="10">
-      <formula>IF(ISBLANK(N2),FALSE,NOT(ISNUMBER(N2)))</formula>
+      <formula>IF(ISBLANK(N2), FALSE, NOT(ISNUMBER(N2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" errorTitle="Invalid value" error="Value must be in list" sqref="J2:J1048576">
-      <formula1>'enum.drill_method'!$A$1:$A$3</formula1>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" errorTitle="Invalid value" error="Value must be in the dropdown list" sqref="J2:J1048576">
+      <formula1>'lists'!$A$1:$A$3</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" errorTitle="Invalid value" error="Value must be TRUE or FALSE" sqref="M2:M1048576">
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" errorTitle="Invalid value" error="Value must be in the dropdown list" sqref="M2:M1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -992,9 +973,9 @@
     <col min="1" max="1" width="13.85546875" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" customWidth="1"/>
-    <col min="4" max="7" width="10.7109375" customWidth="1"/>
+    <col min="4" max="6" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
     <col min="8" max="8" width="15.140625" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1026,39 +1007,39 @@
   </sheetData>
   <conditionalFormatting sqref="A2:A1048576">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>OR(AND(ISBLANK(A2),COUNTBLANK($A2:$H2)&lt;&gt;8),IF(ISBLANK(A2),FALSE,IF(ISNUMBER(A2),INT(A2)&lt;&gt;A2,TRUE)))</formula>
+      <formula>OR(AND(ISBLANK(A2), COUNTBLANK($A2:$H2) &lt;&gt; 8), IF(ISBLANK(A2), FALSE, OR(IF(ISNUMBER(A2), INT(A2) &lt;&gt; A2, TRUE), ISNA(MATCH(A2, 'borehole'!$A$2:$A$1048576, 0)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B1048576">
     <cfRule type="expression" dxfId="0" priority="2">
-      <formula>OR(AND(ISBLANK(B2),COUNTBLANK($A2:$H2)&lt;&gt;8),IF(ISBLANK(B2),FALSE,NOT(ISNUMBER(B2))))</formula>
+      <formula>OR(AND(ISBLANK(B2), COUNTBLANK($A2:$H2) &lt;&gt; 8), IF(ISBLANK(B2), FALSE, NOT(ISNUMBER(B2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C1048576">
     <cfRule type="expression" dxfId="0" priority="3">
-      <formula>OR(AND(ISBLANK(C2),COUNTBLANK($A2:$H2)&lt;&gt;8),IF(ISBLANK(C2),FALSE,NOT(ISNUMBER(C2))))</formula>
+      <formula>OR(AND(ISBLANK(C2), COUNTBLANK($A2:$H2) &lt;&gt; 8), IF(ISBLANK(C2), FALSE, NOT(ISNUMBER(C2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E1048576">
     <cfRule type="expression" dxfId="0" priority="4">
-      <formula>AND(ISBLANK(E2),COUNTBLANK($A2:$H2)&lt;&gt;8)</formula>
+      <formula>AND(ISBLANK(E2), COUNTBLANK($A2:$H2) &lt;&gt; 8)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G1048576">
     <cfRule type="expression" dxfId="0" priority="5">
-      <formula>IF(ISBLANK(G2),FALSE,AND(G2&lt;&gt;TRUE,G2&lt;&gt;FALSE))</formula>
+      <formula>IF(ISBLANK(G2), FALSE, NOT(ISNUMBER(G2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H1048576">
     <cfRule type="expression" dxfId="0" priority="6">
-      <formula>IF(ISBLANK(H2),FALSE,AND(H2&lt;&gt;TRUE,H2&lt;&gt;FALSE))</formula>
+      <formula>IF(ISBLANK(H2), FALSE, AND(H2 &lt;&gt; TRUE, H2 &lt;&gt; FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" errorTitle="Invalid value" error="Value must be TRUE or FALSE" sqref="G2:G1048576">
-      <formula1>"TRUE,FALSE"</formula1>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" errorTitle="Invalid value" error="Value must be in the dropdown list" sqref="A2:A1048576">
+      <formula1>'borehole'!$A$2:$A$1048576</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" errorTitle="Invalid value" error="Value must be TRUE or FALSE" sqref="H2:H1048576">
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" errorTitle="Invalid value" error="Value must be in the dropdown list" sqref="H2:H1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1091,7 +1072,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>